<commit_message>
add canonical to be as decided in point interop (#17) 7041af722d2b54bb31ba7942346825819640647e
</commit_message>
<xml_diff>
--- a/ig/main/StructureDefinition-ror-accessibility-location.xlsx
+++ b/ig/main/StructureDefinition-ror-accessibility-location.xlsx
@@ -24,7 +24,7 @@
     <t>URL</t>
   </si>
   <si>
-    <t>http://interop.esante.gouv.fr/fhir/ig/ror24/StructureDefinition/ror-accessibility-location</t>
+    <t>http://interop.esante.gouv.fr/ig/fhir/ror24/StructureDefinition/ror-accessibility-location</t>
   </si>
   <si>
     <t>Version</t>
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-02-21T16:28:41+00:00</t>
+    <t>2023-02-22T09:44:01+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
replace http to https and fix ig/fhir forgotten change (#21) 0cfdf83211cd73a59b4ecfc7cafcf9f321c200b5
</commit_message>
<xml_diff>
--- a/ig/main/StructureDefinition-ror-accessibility-location.xlsx
+++ b/ig/main/StructureDefinition-ror-accessibility-location.xlsx
@@ -24,7 +24,7 @@
     <t>URL</t>
   </si>
   <si>
-    <t>http://interop.esante.gouv.fr/ig/fhir/ror24/StructureDefinition/ror-accessibility-location</t>
+    <t>https://interop.esante.gouv.fr/ig/fhir/ror24/StructureDefinition/ror-accessibility-location</t>
   </si>
   <si>
     <t>Version</t>
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-02-24T16:23:59+00:00</t>
+    <t>2023-02-27T11:21:32+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>